<commit_message>
libreta de graficas, grafica por nacionalidades, correcion de error en get-data
</commit_message>
<xml_diff>
--- a/notebooks/aspirantes-mcd.xlsx
+++ b/notebooks/aspirantes-mcd.xlsx
@@ -588,7 +588,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -766,7 +766,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>35</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1081,7 +1081,7 @@
         <v>38</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1126,7 +1126,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1169,7 +1169,7 @@
         <v>37</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1255,7 +1255,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1746,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1834,7 +1834,7 @@
         <v>31</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1879,7 +1879,7 @@
         <v>31</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>44</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2014,7 +2014,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2059,7 +2059,7 @@
         <v>32</v>
       </c>
       <c r="D37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2104,7 +2104,7 @@
         <v>36</v>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2149,7 +2149,7 @@
         <v>29</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2194,7 +2194,7 @@
         <v>35</v>
       </c>
       <c r="D40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2239,7 +2239,7 @@
         <v>31</v>
       </c>
       <c r="D41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>30</v>
       </c>
       <c r="D42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2329,7 +2329,7 @@
         <v>34</v>
       </c>
       <c r="D43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         <v>34</v>
       </c>
       <c r="D44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2419,7 +2419,7 @@
         <v>36</v>
       </c>
       <c r="D45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2464,7 +2464,7 @@
         <v>34</v>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2509,7 +2509,7 @@
         <v>32</v>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         <v>34</v>
       </c>
       <c r="D49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2644,7 +2644,7 @@
         <v>26</v>
       </c>
       <c r="D50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2689,7 +2689,7 @@
         <v>33</v>
       </c>
       <c r="D51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2732,7 +2732,7 @@
         <v>48</v>
       </c>
       <c r="D52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2777,7 +2777,7 @@
         <v>42</v>
       </c>
       <c r="D53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>26</v>
       </c>
       <c r="D55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         <v>39</v>
       </c>
       <c r="D56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2955,7 +2955,7 @@
         <v>24</v>
       </c>
       <c r="D57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3000,7 +3000,7 @@
         <v>26</v>
       </c>
       <c r="D58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
         <v>37</v>
       </c>
       <c r="D59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3088,7 +3088,7 @@
         <v>25</v>
       </c>
       <c r="D60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3133,7 +3133,7 @@
         <v>41</v>
       </c>
       <c r="D61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
         <v>29</v>
       </c>
       <c r="D62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3223,7 +3223,7 @@
         <v>42</v>
       </c>
       <c r="D63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -3268,7 +3268,7 @@
         <v>34</v>
       </c>
       <c r="D64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3313,7 +3313,7 @@
         <v>44</v>
       </c>
       <c r="D65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3358,7 +3358,7 @@
         <v>42</v>
       </c>
       <c r="D66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
         <v>32</v>
       </c>
       <c r="D67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3448,7 +3448,7 @@
         <v>27</v>
       </c>
       <c r="D68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3493,7 +3493,7 @@
         <v>28</v>
       </c>
       <c r="D69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
         <v>25</v>
       </c>
       <c r="D70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3581,7 +3581,7 @@
         <v>31</v>
       </c>
       <c r="D71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3626,7 +3626,7 @@
         <v>26</v>
       </c>
       <c r="D72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3671,7 +3671,7 @@
         <v>32</v>
       </c>
       <c r="D73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3716,7 +3716,7 @@
         <v>25</v>
       </c>
       <c r="D74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3747,7 +3747,7 @@
         <v>27</v>
       </c>
       <c r="D75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3792,7 +3792,7 @@
         <v>31</v>
       </c>
       <c r="D76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
         <v>27</v>
       </c>
       <c r="D77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3882,7 +3882,7 @@
         <v>29</v>
       </c>
       <c r="D78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
         <v>26</v>
       </c>
       <c r="D79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4017,7 +4017,7 @@
         <v>26</v>
       </c>
       <c r="D81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4062,7 +4062,7 @@
         <v>28</v>
       </c>
       <c r="D82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
         <v>25</v>
       </c>
       <c r="D85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4273,7 +4273,7 @@
         <v>26</v>
       </c>
       <c r="D87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -4363,7 +4363,7 @@
         <v>25</v>
       </c>
       <c r="D89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4588,7 +4588,7 @@
         <v>39</v>
       </c>
       <c r="D94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4633,7 +4633,7 @@
         <v>29</v>
       </c>
       <c r="D95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4723,7 +4723,7 @@
         <v>29</v>
       </c>
       <c r="D97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4768,7 +4768,7 @@
         <v>47</v>
       </c>
       <c r="D98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
         <v>39</v>
       </c>
       <c r="D99" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4903,7 +4903,7 @@
         <v>25</v>
       </c>
       <c r="D101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4993,7 +4993,7 @@
         <v>34</v>
       </c>
       <c r="D103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5038,7 +5038,7 @@
         <v>23</v>
       </c>
       <c r="D104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -5081,7 +5081,7 @@
         <v>24</v>
       </c>
       <c r="D105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5126,7 +5126,7 @@
         <v>30</v>
       </c>
       <c r="D106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5169,7 +5169,7 @@
         <v>27</v>
       </c>
       <c r="D107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -5214,7 +5214,7 @@
         <v>25</v>
       </c>
       <c r="D108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -5302,7 +5302,7 @@
         <v>30</v>
       </c>
       <c r="D110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -5392,7 +5392,7 @@
         <v>24</v>
       </c>
       <c r="D112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5435,7 +5435,7 @@
         <v>25</v>
       </c>
       <c r="D113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5478,7 +5478,7 @@
         <v>41</v>
       </c>
       <c r="D114" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -5568,7 +5568,7 @@
         <v>60</v>
       </c>
       <c r="D116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -5611,7 +5611,7 @@
         <v>60</v>
       </c>
       <c r="D117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -5656,7 +5656,7 @@
         <v>60</v>
       </c>
       <c r="D118" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -5699,7 +5699,7 @@
         <v>60</v>
       </c>
       <c r="D119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -5742,7 +5742,7 @@
         <v>60</v>
       </c>
       <c r="D120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -5875,7 +5875,7 @@
         <v>27</v>
       </c>
       <c r="D123" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5920,7 +5920,7 @@
         <v>31</v>
       </c>
       <c r="D124" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5965,7 +5965,7 @@
         <v>31</v>
       </c>
       <c r="D125" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6100,7 +6100,7 @@
         <v>21</v>
       </c>
       <c r="D128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6145,7 +6145,7 @@
         <v>25</v>
       </c>
       <c r="D129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -6280,7 +6280,7 @@
         <v>28</v>
       </c>
       <c r="D132" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6325,7 +6325,7 @@
         <v>30</v>
       </c>
       <c r="D133" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6415,7 +6415,7 @@
         <v>30</v>
       </c>
       <c r="D135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -6460,7 +6460,7 @@
         <v>24</v>
       </c>
       <c r="D136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -6550,7 +6550,7 @@
         <v>31</v>
       </c>
       <c r="D138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -6640,7 +6640,7 @@
         <v>23</v>
       </c>
       <c r="D140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -6685,7 +6685,7 @@
         <v>25</v>
       </c>
       <c r="D141" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -6730,7 +6730,7 @@
         <v>32</v>
       </c>
       <c r="D142" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -6775,7 +6775,7 @@
         <v>27</v>
       </c>
       <c r="D143" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -6820,7 +6820,7 @@
         <v>25</v>
       </c>
       <c r="D144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -6863,7 +6863,7 @@
         <v>57</v>
       </c>
       <c r="D145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -6908,7 +6908,7 @@
         <v>27</v>
       </c>
       <c r="D146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7043,7 +7043,7 @@
         <v>27</v>
       </c>
       <c r="D149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7088,7 +7088,7 @@
         <v>30</v>
       </c>
       <c r="D150" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7133,7 +7133,7 @@
         <v>25</v>
       </c>
       <c r="D151" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7178,7 +7178,7 @@
         <v>26</v>
       </c>
       <c r="D152" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -7223,7 +7223,7 @@
         <v>28</v>
       </c>
       <c r="D153" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7268,7 +7268,7 @@
         <v>26</v>
       </c>
       <c r="D154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7358,7 +7358,7 @@
         <v>27</v>
       </c>
       <c r="D156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -7448,7 +7448,7 @@
         <v>34</v>
       </c>
       <c r="D158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
         <v>33</v>
       </c>
       <c r="D160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -7673,7 +7673,7 @@
         <v>28</v>
       </c>
       <c r="D163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -7716,7 +7716,7 @@
         <v>26</v>
       </c>
       <c r="D164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -7851,7 +7851,7 @@
         <v>24</v>
       </c>
       <c r="D167" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -7896,7 +7896,7 @@
         <v>22</v>
       </c>
       <c r="D168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -7939,7 +7939,7 @@
         <v>22</v>
       </c>
       <c r="D169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8027,7 +8027,7 @@
         <v>37</v>
       </c>
       <c r="D171" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -8072,7 +8072,7 @@
         <v>27</v>
       </c>
       <c r="D172" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -8117,7 +8117,7 @@
         <v>29</v>
       </c>
       <c r="D173" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -8162,7 +8162,7 @@
         <v>29</v>
       </c>
       <c r="D174" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -8283,7 +8283,7 @@
         <v>40</v>
       </c>
       <c r="D177" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -8328,7 +8328,7 @@
         <v>24</v>
       </c>
       <c r="D178" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -8373,7 +8373,7 @@
         <v>29</v>
       </c>
       <c r="D179" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -8463,7 +8463,7 @@
         <v>26</v>
       </c>
       <c r="D181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -8598,7 +8598,7 @@
         <v>30</v>
       </c>
       <c r="D184" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -8643,7 +8643,7 @@
         <v>33</v>
       </c>
       <c r="D185" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -8823,7 +8823,7 @@
         <v>25</v>
       </c>
       <c r="D189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -8911,7 +8911,7 @@
         <v>27</v>
       </c>
       <c r="D191" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -8956,7 +8956,7 @@
         <v>24</v>
       </c>
       <c r="D192" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -9001,7 +9001,7 @@
         <v>45</v>
       </c>
       <c r="D193" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -9046,7 +9046,7 @@
         <v>23</v>
       </c>
       <c r="D194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -9091,7 +9091,7 @@
         <v>26</v>
       </c>
       <c r="D195" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -9136,7 +9136,7 @@
         <v>32</v>
       </c>
       <c r="D196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9181,7 +9181,7 @@
         <v>34</v>
       </c>
       <c r="D197" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9226,7 +9226,7 @@
         <v>24</v>
       </c>
       <c r="D198" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         <v>25</v>
       </c>
       <c r="D199" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -9312,7 +9312,7 @@
         <v>25</v>
       </c>
       <c r="D200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -9357,7 +9357,7 @@
         <v>25</v>
       </c>
       <c r="D201" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -9402,7 +9402,7 @@
         <v>28</v>
       </c>
       <c r="D202" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -9447,7 +9447,7 @@
         <v>32</v>
       </c>
       <c r="D203" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -9492,7 +9492,7 @@
         <v>29</v>
       </c>
       <c r="D204" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -9537,7 +9537,7 @@
         <v>27</v>
       </c>
       <c r="D205" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -9582,7 +9582,7 @@
         <v>24</v>
       </c>
       <c r="D206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -9627,7 +9627,7 @@
         <v>23</v>
       </c>
       <c r="D207" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -9717,7 +9717,7 @@
         <v>27</v>
       </c>
       <c r="D209" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -9807,7 +9807,7 @@
         <v>25</v>
       </c>
       <c r="D211" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -9852,7 +9852,7 @@
         <v>23</v>
       </c>
       <c r="D212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -9895,7 +9895,7 @@
         <v>32</v>
       </c>
       <c r="D213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -9985,7 +9985,7 @@
         <v>26</v>
       </c>
       <c r="D215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10028,7 +10028,7 @@
         <v>24</v>
       </c>
       <c r="D216" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -10073,7 +10073,7 @@
         <v>23</v>
       </c>
       <c r="D217" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10163,7 +10163,7 @@
         <v>28</v>
       </c>
       <c r="D219" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10253,7 +10253,7 @@
         <v>23</v>
       </c>
       <c r="D221" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -10296,7 +10296,7 @@
         <v>24</v>
       </c>
       <c r="D222" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -10341,7 +10341,7 @@
         <v>25</v>
       </c>
       <c r="D223" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -10386,7 +10386,7 @@
         <v>37</v>
       </c>
       <c r="D224" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -10431,7 +10431,7 @@
         <v>25</v>
       </c>
       <c r="D225" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -10476,7 +10476,7 @@
         <v>32</v>
       </c>
       <c r="D226" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -10566,7 +10566,7 @@
         <v>37</v>
       </c>
       <c r="D228" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -10611,7 +10611,7 @@
         <v>25</v>
       </c>
       <c r="D229" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -10656,7 +10656,7 @@
         <v>36</v>
       </c>
       <c r="D230" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -10746,7 +10746,7 @@
         <v>22</v>
       </c>
       <c r="D232" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -10791,7 +10791,7 @@
         <v>26</v>
       </c>
       <c r="D233" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -10834,7 +10834,7 @@
         <v>39</v>
       </c>
       <c r="D234" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -10879,7 +10879,7 @@
         <v>26</v>
       </c>
       <c r="D235" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -10924,7 +10924,7 @@
         <v>30</v>
       </c>
       <c r="D236" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -10969,7 +10969,7 @@
         <v>23</v>
       </c>
       <c r="D237" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -11057,7 +11057,7 @@
         <v>28</v>
       </c>
       <c r="D239" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -11102,7 +11102,7 @@
         <v>28</v>
       </c>
       <c r="D240" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11147,7 +11147,7 @@
         <v>23</v>
       </c>
       <c r="D241" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>

</xml_diff>